<commit_message>
Old version of template... Change to the correct one
</commit_message>
<xml_diff>
--- a/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
+++ b/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Etk-git\TestsAndDemos\Etk.Tests.Templates.ExcelDna1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8040"/>
   </bookViews>
@@ -24,8 +19,8 @@
     <definedName name="DEC_STATUS">'Dashboard Templates'!$A$20:$A$21</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,7 +33,7 @@
     <author>BlouinSide</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0">
+    <comment ref="C10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0" shapeId="0">
+    <comment ref="E13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B28" authorId="0" shapeId="0">
+    <comment ref="B28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -276,12 +271,6 @@
     <t>Surname</t>
   </si>
   <si>
-    <t>{R:Forename}</t>
-  </si>
-  <si>
-    <t>{R:Surname}</t>
-  </si>
-  <si>
     <t>{{{Forename} {Surname}}}</t>
   </si>
   <si>
@@ -306,12 +295,6 @@
     <t>&lt;Link To='Orders1' With='GetOrders' /&gt;</t>
   </si>
   <si>
-    <t>{R:Id}</t>
-  </si>
-  <si>
-    <t>{R:Date}</t>
-  </si>
-  <si>
     <t>&lt;Link To='OrderLines1' With='Lines'/&gt;</t>
   </si>
   <si>
@@ -321,12 +304,6 @@
     <t>&lt;Template Name='OrderLines1' BindingWith='OrderLine,Etk.Tests.Data.Services' /&gt;</t>
   </si>
   <si>
-    <t>{R:Product.Name}</t>
-  </si>
-  <si>
-    <t>{R:Product.UnitPrice}</t>
-  </si>
-  <si>
     <t>{Quantity}</t>
   </si>
   <si>
@@ -339,9 +316,6 @@
     <t>Product Name</t>
   </si>
   <si>
-    <t>{R:Product.Id}</t>
-  </si>
-  <si>
     <t>&lt;Template Name='ShopCustomers'  BindingWith='Customer'/&gt;</t>
   </si>
   <si>
@@ -357,9 +331,6 @@
     <t>{Price}</t>
   </si>
   <si>
-    <t>&lt;NR Name='Id_{Id}'&gt;{R:Id}&lt;/NR&gt;</t>
-  </si>
-  <si>
     <t>&lt;NR Name='Vertt_[POS]'&gt;{Id}&lt;/NR&gt;</t>
   </si>
   <si>
@@ -426,24 +397,9 @@
     <t>DEC_DONE</t>
   </si>
   <si>
-    <t>{DEC=DEC_STATUS:Status}</t>
-  </si>
-  <si>
-    <t>{DEC=DEC_DONE:Done}</t>
-  </si>
-  <si>
-    <t>{DEC=DEC_EXEC:Success}</t>
-  </si>
-  <si>
     <t>&lt;Template Name='Main' BindingWith='ExcelTestsManager'/&gt;</t>
   </si>
   <si>
-    <t>{ME=ExcelTestTopic,,GetNumberOfTests;LDC=ExcelTestsManager,Etk.Tests.Templates.ExcelDna1,SetSearchValue:Description}</t>
-  </si>
-  <si>
-    <t>{LDC=ExcelTest,Etk.Tests.Templates.ExcelDna1,DisplayResultSheet:Description}</t>
-  </si>
-  <si>
     <t>&lt;Template Name='TestTopics' BindingWith='IExcelTestTopic' /&gt;</t>
   </si>
   <si>
@@ -459,12 +415,6 @@
     <t>&lt;Template Name='Products' BindingWith='Product' /&gt;</t>
   </si>
   <si>
-    <t>{R:Name}</t>
-  </si>
-  <si>
-    <t>{R:UnitPrice}</t>
-  </si>
-  <si>
     <t>&lt;EndTemplate Name='Products'/&gt;</t>
   </si>
   <si>
@@ -486,9 +436,6 @@
     <t>&lt;EndTemplate Name='BasicVerticalMultiHeaderAndFooter'/&gt;</t>
   </si>
   <si>
-    <t>{ME=ExcelTestTopic,Etk.Tests.Templates.ExcelDna1,GetNumberOfTests;DEC=DEC_INIT:RenderSuccessful}</t>
-  </si>
-  <si>
     <t>Go back to Dashboard template</t>
   </si>
   <si>
@@ -498,18 +445,9 @@
     <t>&lt;Template Name='GoBackToDashboard' BindingWith='GoBackToDashBoardManager'/&gt;</t>
   </si>
   <si>
-    <t>[LDC=,,GoBackToDashboard:Go back to dashboard]</t>
-  </si>
-  <si>
     <t>Init Ok</t>
   </si>
   <si>
-    <t>[LDC=ExcelTestsManager,,Execute:Execute All Tests]</t>
-  </si>
-  <si>
-    <t>[ME=ExcelTestTopic,,GetNumberOfTests;LDC=,,Execute:Execute]</t>
-  </si>
-  <si>
     <t>Tests data  binding</t>
   </si>
   <si>
@@ -568,13 +506,70 @@
   </si>
   <si>
     <t>&lt;Link To='ShopCustomers' With='Customers' /&gt;</t>
+  </si>
+  <si>
+    <t>{R::Id}</t>
+  </si>
+  <si>
+    <t>{R::Name}</t>
+  </si>
+  <si>
+    <t>{R::UnitPrice}</t>
+  </si>
+  <si>
+    <t>&lt;NR Name='Id_{Id}'&gt;{R::Id}&lt;/NR&gt;</t>
+  </si>
+  <si>
+    <t>{R::Forename}</t>
+  </si>
+  <si>
+    <t>{R::Surname}</t>
+  </si>
+  <si>
+    <t>{R::Date}</t>
+  </si>
+  <si>
+    <t>{R::Product.Id}</t>
+  </si>
+  <si>
+    <t>{R::Product.Name}</t>
+  </si>
+  <si>
+    <t>{R::Product.UnitPrice}</t>
+  </si>
+  <si>
+    <t>{DEC=DEC_STATUS::Status}</t>
+  </si>
+  <si>
+    <t>[LDC=ExcelTestsManager,,Execute::Execute All Tests]</t>
+  </si>
+  <si>
+    <t>[ME=ExcelTestTopic,,GetNumberOfTests;LDC=,,Execute::Execute]</t>
+  </si>
+  <si>
+    <t>{ME=ExcelTestTopic,,GetNumberOfTests;LDC=ExcelTestsManager,Etk.Tests.Templates.ExcelDna1,SetSearchValue::Description}</t>
+  </si>
+  <si>
+    <t>{ME=ExcelTestTopic,Etk.Tests.Templates.ExcelDna1,GetNumberOfTests;DEC=DEC_INIT::RenderSuccessful}</t>
+  </si>
+  <si>
+    <t>{LDC=ExcelTest,Etk.Tests.Templates.ExcelDna1,DisplayResultSheet::Description}</t>
+  </si>
+  <si>
+    <t>{DEC=DEC_DONE::Done}</t>
+  </si>
+  <si>
+    <t>{DEC=DEC_EXEC::Success}</t>
+  </si>
+  <si>
+    <t>[LDC=,,GoBackToDashboard::Go back to dashboard]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1522,21 +1517,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="N2:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="28"/>
     <col min="2" max="2" width="15.85546875" style="28" customWidth="1"/>
@@ -1554,7 +1549,7 @@
     <col min="16" max="16384" width="11.42578125" style="28"/>
   </cols>
   <sheetData>
-    <row r="2" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="14:15">
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
     </row>
@@ -1566,17 +1561,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="85.28515625" customWidth="1"/>
@@ -1592,12 +1587,12 @@
     <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="28"/>
     </row>
-    <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="21">
       <c r="A3" s="40" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -1615,52 +1610,52 @@
       <c r="O3" s="41"/>
       <c r="P3" s="42"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>94</v>
+        <v>133</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15.75" thickBot="1">
       <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="B7" s="28" t="s">
         <v>78</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
-        <v>86</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
@@ -1668,104 +1663,104 @@
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I7" s="28"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="B10" s="31" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="D12" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="E13" s="25" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1">
       <c r="A18" s="43" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
       <c r="D18" s="44"/>
     </row>
-    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15.75" thickBot="1">
       <c r="A19" s="36" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="37" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="38" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="21">
       <c r="A25" s="40" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
@@ -1783,17 +1778,17 @@
       <c r="O25" s="41"/>
       <c r="P25" s="42"/>
     </row>
-    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15.75" thickBot="1">
       <c r="A27" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" thickBot="1">
       <c r="B28" s="35" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1809,7 +1804,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
@@ -1817,10 +1812,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:19" ht="21.75" thickBot="1">
       <c r="A3" s="45" t="s">
         <v>25</v>
       </c>
@@ -1840,7 +1835,7 @@
       <c r="O3" s="46"/>
       <c r="P3" s="47"/>
     </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1858,7 +1853,7 @@
       <c r="R5" s="49"/>
       <c r="S5" s="50"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1876,7 +1871,7 @@
       <c r="R6" s="52"/>
       <c r="S6" s="53"/>
     </row>
-    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="15" customHeight="1">
       <c r="I7" s="54" t="s">
         <v>26</v>
       </c>
@@ -1891,7 +1886,7 @@
       <c r="R7" s="55"/>
       <c r="S7" s="56"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1909,7 +1904,7 @@
       <c r="R10" s="49"/>
       <c r="S10" s="50"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1927,7 +1922,7 @@
       <c r="R11" s="52"/>
       <c r="S11" s="53"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="I12" s="54" t="s">
         <v>26</v>
       </c>
@@ -1942,7 +1937,7 @@
       <c r="R12" s="55"/>
       <c r="S12" s="56"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1960,7 +1955,7 @@
       <c r="R15" s="49"/>
       <c r="S15" s="50"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="I16" s="51"/>
       <c r="J16" s="52"/>
       <c r="K16" s="52"/>
@@ -1973,7 +1968,7 @@
       <c r="R16" s="52"/>
       <c r="S16" s="53"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="15" customHeight="1">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1989,12 +1984,12 @@
       <c r="R17" s="55"/>
       <c r="S17" s="56"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="15" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -2015,7 +2010,7 @@
       <c r="R21" s="49"/>
       <c r="S21" s="50"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="I22" s="51"/>
       <c r="J22" s="52"/>
       <c r="K22" s="52"/>
@@ -2028,7 +2023,7 @@
       <c r="R22" s="52"/>
       <c r="S22" s="53"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="15" customHeight="1">
       <c r="C23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2062,7 +2057,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
@@ -2072,7 +2067,7 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
@@ -2083,9 +2078,9 @@
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="21">
       <c r="A3" s="40" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -2103,7 +2098,7 @@
       <c r="O3" s="41"/>
       <c r="P3" s="42"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="60" t="s">
         <v>0</v>
       </c>
@@ -2123,12 +2118,12 @@
       <c r="O4" s="61"/>
       <c r="P4" s="62"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
@@ -2145,7 +2140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="60" t="s">
         <v>2</v>
       </c>
@@ -2165,12 +2160,12 @@
       <c r="O8" s="61"/>
       <c r="P8" s="62"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2187,7 +2182,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>28</v>
@@ -2202,7 +2197,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -2216,7 +2211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="60" t="s">
         <v>6</v>
       </c>
@@ -2236,12 +2231,12 @@
       <c r="O15" s="61"/>
       <c r="P15" s="62"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -2252,7 +2247,7 @@
       <c r="D17" s="64"/>
       <c r="E17" s="65"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2269,10 +2264,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>29</v>
@@ -2284,7 +2279,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -2295,7 +2290,7 @@
       <c r="D20" s="64"/>
       <c r="E20" s="65"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -2306,12 +2301,12 @@
       <c r="D21" s="64"/>
       <c r="E21" s="65"/>
       <c r="F21" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="21">
       <c r="A26" s="40" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
@@ -2329,9 +2324,9 @@
       <c r="O26" s="41"/>
       <c r="P26" s="42"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16">
       <c r="A27" s="60" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B27" s="61"/>
       <c r="C27" s="61"/>
@@ -2349,9 +2344,9 @@
       <c r="O27" s="61"/>
       <c r="P27" s="62"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16">
       <c r="A29" s="1" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -2363,13 +2358,13 @@
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16">
       <c r="A30" s="1"/>
       <c r="B30" s="4" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
@@ -2381,7 +2376,7 @@
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16">
       <c r="A31" s="1"/>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
@@ -2393,9 +2388,9 @@
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16">
       <c r="A32" s="60" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B32" s="61"/>
       <c r="C32" s="61"/>
@@ -2413,9 +2408,9 @@
       <c r="O32" s="61"/>
       <c r="P32" s="62"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17">
       <c r="A33" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B33" s="63" t="s">
         <v>37</v>
@@ -2426,7 +2421,7 @@
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17">
       <c r="A34" s="1"/>
       <c r="B34" s="3" t="s">
         <v>31</v>
@@ -2450,7 +2445,7 @@
       <c r="M34" s="15"/>
       <c r="N34" s="15"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17">
       <c r="B35" s="2" t="s">
         <v>28</v>
       </c>
@@ -2473,9 +2468,9 @@
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17">
       <c r="B36" s="66" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C36" s="67"/>
       <c r="D36" s="67"/>
@@ -2489,15 +2484,15 @@
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17">
       <c r="B37" s="4" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
       <c r="G37" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
@@ -2506,13 +2501,13 @@
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17">
       <c r="A38" s="1"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17">
       <c r="A39" s="1"/>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
@@ -2524,9 +2519,9 @@
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17">
       <c r="A40" s="60" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B40" s="61"/>
       <c r="C40" s="61"/>
@@ -2544,9 +2539,9 @@
       <c r="O40" s="61"/>
       <c r="P40" s="62"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17">
       <c r="A41" s="4" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2561,19 +2556,19 @@
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17">
       <c r="A42" s="4"/>
       <c r="B42" s="11" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
@@ -2583,12 +2578,12 @@
       <c r="M42" s="15"/>
       <c r="N42" s="15"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17">
       <c r="A43" s="1"/>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17">
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -2599,9 +2594,9 @@
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17">
       <c r="A45" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2618,7 +2613,7 @@
       <c r="N45" s="15"/>
       <c r="O45" s="15"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17">
       <c r="B46" s="21" t="s">
         <v>39</v>
       </c>
@@ -2635,22 +2630,22 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17">
       <c r="B47" s="17"/>
       <c r="C47" s="18" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="D47" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E47" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:17">
       <c r="B48" s="8" t="s">
         <v>33</v>
       </c>
@@ -2661,11 +2656,11 @@
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
       <c r="G48" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="K48" s="4"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
       <c r="D49" s="16"/>
@@ -2673,12 +2668,12 @@
       <c r="F49" s="16"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="A51" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2688,31 +2683,31 @@
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="A52" s="4"/>
       <c r="B52" s="9" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11">
       <c r="G54" s="4"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11">
       <c r="A55" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2720,30 +2715,30 @@
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11">
       <c r="A56" s="4"/>
       <c r="B56" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E56" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2751,22 +2746,22 @@
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11">
       <c r="A59" s="4"/>
       <c r="B59" s="11" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="57" t="s">
         <v>40</v>
       </c>
@@ -2778,43 +2773,43 @@
       <c r="G69" s="58"/>
       <c r="H69" s="59"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="F70" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D70" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E70" s="6" t="s">
+      <c r="G70" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F70" s="6" t="s">
+      <c r="H70" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G70" s="6" t="s">
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="16" t="s">
         <v>51</v>
-      </c>
-      <c r="H70" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
-        <v>53</v>
       </c>
       <c r="C71" s="15"/>
       <c r="F71" s="16"/>
       <c r="G71" s="16"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2841,7 +2836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
@@ -2851,11 +2846,11 @@
       <selection activeCell="B6" sqref="B6:O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="21">
       <c r="A2" s="40" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -2873,9 +2868,9 @@
       <c r="O2" s="41"/>
       <c r="P2" s="42"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="60" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B4" s="61"/>
       <c r="C4" s="61"/>
@@ -2893,56 +2888,56 @@
       <c r="O4" s="61"/>
       <c r="P4" s="62"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="B6" s="2" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct a few bugs. Testing Etk with Excel 2016
</commit_message>
<xml_diff>
--- a/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
+++ b/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rblouin051512\USERS\perso\Etk\ETK-GitHub\Tests\Etk.Tests.Templates.ExcelDna1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8040"/>
   </bookViews>
@@ -12,15 +17,24 @@
     <sheet name="BadTemplates" sheetId="3" r:id="rId3"/>
     <sheet name="BasicTemplates1" sheetId="1" r:id="rId4"/>
     <sheet name="DataBindingTemplates" sheetId="6" r:id="rId5"/>
+    <sheet name="VerticalNoHeaderAndFooter" sheetId="7" r:id="rId6"/>
+    <sheet name="VerticalMonoHeaderAndFooter" sheetId="8" r:id="rId7"/>
+    <sheet name="VerticalMultiHeaderAndFooter" sheetId="9" r:id="rId8"/>
+    <sheet name="VerticalWithOnlyOneLink" sheetId="10" r:id="rId9"/>
+    <sheet name="BasicEtkFeatures" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="DEC_DONE">'Dashboard Templates'!$C$20:$C$21</definedName>
     <definedName name="DEC_EXEC">'Dashboard Templates'!$D$20:$D$21</definedName>
     <definedName name="DEC_STATUS">'Dashboard Templates'!$A$20:$A$21</definedName>
+    <definedName name="Vertt_0" localSheetId="7">VerticalMultiHeaderAndFooter!$B$5</definedName>
+    <definedName name="Vertt_1" localSheetId="7">VerticalMultiHeaderAndFooter!$B$6</definedName>
+    <definedName name="Vertt_2" localSheetId="7">VerticalMultiHeaderAndFooter!$B$7</definedName>
+    <definedName name="Vertt_3" localSheetId="7">VerticalMultiHeaderAndFooter!$B$8</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +47,7 @@
     <author>BlouinSide</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -95,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +122,492 @@
         </r>
       </text>
     </comment>
-    <comment ref="B28" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to execute the concerned tests</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to filter the view on this test topic.
+Double left clic again to remove the filter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to display the sheet we are testing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to display the sheet we are testing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to execute the concerned tests</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to filter the view on this test topic.
+Double left clic again to remove the filter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to display the sheet we are testing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to display the sheet we are testing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to execute the concerned tests</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to filter the view on this test topic.
+Double left clic again to remove the filter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to display the sheet we are testing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to execute the concerned tests</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to filter the view on this test topic.
+Double left clic again to remove the filter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to display the sheet we are testing.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>BlouinSide</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to execute all tests</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to execute the concerned tests</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to filter the view on this test topic.
+Double left clic again to remove the filter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to display the sheet we are testing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to go back to the dashboard</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>BlouinSide</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to go back to the dashboard</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>BlouinSide</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to go back to the dashboard</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>BlouinSide</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to go back to the dashboard</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>BlouinSide</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to go back to the dashboard</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>BlouinSide</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -137,7 +636,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="177">
   <si>
     <t>Template without header and footer</t>
   </si>
@@ -563,13 +1062,118 @@
   </si>
   <si>
     <t>[LDC=,,GoBackToDashboard::Go back to dashboard]</t>
+  </si>
+  <si>
+    <t>Go back to dashboard</t>
+  </si>
+  <si>
+    <t>Search...</t>
+  </si>
+  <si>
+    <t>Execute All Tests</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>Tests on a basic template without linked templates and without header or footer</t>
+  </si>
+  <si>
+    <t>Control the size of the rendered area and the value of some cells</t>
+  </si>
+  <si>
+    <t>Tests on a basic template (without linked templates) with a one line header and a one line footer</t>
+  </si>
+  <si>
+    <t>Check the rendering of the template parts</t>
+  </si>
+  <si>
+    <t>Tests on a basic template (without linked templates) with a 2 lines header and 2 lines footer</t>
+  </si>
+  <si>
+    <t>Control the size of the rendered area of the template parts and the value of some cells of these template parts</t>
+  </si>
+  <si>
+    <t>Tests on a basic template with nothing else than one linked template</t>
+  </si>
+  <si>
+    <t>Tests basic ETK features</t>
+  </si>
+  <si>
+    <t>Try to render after a first rendering with no clear or SetDataSource between</t>
+  </si>
+  <si>
+    <t>First Shop</t>
+  </si>
+  <si>
+    <t>1 Shops Road ShopCity</t>
+  </si>
+  <si>
+    <t>First Shop Reception Phone number</t>
+  </si>
+  <si>
+    <t>Second Shop</t>
+  </si>
+  <si>
+    <t>2 Shops Road ShopCity</t>
+  </si>
+  <si>
+    <t>Second Shop Reception Phone number</t>
+  </si>
+  <si>
+    <t>Third Shop</t>
+  </si>
+  <si>
+    <t>3 Shops Road ShopCity</t>
+  </si>
+  <si>
+    <t>Third Shop Reception Phone number</t>
+  </si>
+  <si>
+    <t>Fourth Shop</t>
+  </si>
+  <si>
+    <t>4 No Customer Shops Road ShopCity</t>
+  </si>
+  <si>
+    <t>Fourth Shop Reception Phone number</t>
+  </si>
+  <si>
+    <t>Product 1</t>
+  </si>
+  <si>
+    <t>Product 2</t>
+  </si>
+  <si>
+    <t>Product 3</t>
+  </si>
+  <si>
+    <t>Product 4</t>
+  </si>
+  <si>
+    <t>Product 5</t>
+  </si>
+  <si>
+    <t>Product 6</t>
+  </si>
+  <si>
+    <t>Product 7</t>
+  </si>
+  <si>
+    <t>Product 8</t>
+  </si>
+  <si>
+    <t>Product 9</t>
+  </si>
+  <si>
+    <t>Product 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -633,8 +1237,22 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,8 +1413,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray0625">
+        <fgColor rgb="FF696969"/>
+        <bgColor theme="8" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray0625">
+        <fgColor rgb="FF696969"/>
+        <bgColor theme="9" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF375623"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1038,11 +1686,120 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1238,6 +1995,129 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1517,29 +2397,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="N2:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="28"/>
-    <col min="2" max="2" width="15.85546875" style="28" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.28515625" style="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="28" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="28" customWidth="1"/>
-    <col min="6" max="6" width="100.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="28" customWidth="1"/>
+    <col min="5" max="5" width="101.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" style="28" customWidth="1"/>
     <col min="9" max="9" width="6.140625" style="28" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" style="28" bestFit="1" customWidth="1"/>
@@ -1549,20 +2430,266 @@
     <col min="16" max="16384" width="11.42578125" style="28"/>
   </cols>
   <sheetData>
-    <row r="2" spans="14:15">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="71"/>
+      <c r="C1" s="72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="85" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="87" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="88" t="s">
+        <v>72</v>
+      </c>
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
     </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="75" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="97" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="96" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="77" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="78" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="98" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" s="96" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="79"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="96" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="77" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="78" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="98" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="96" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="79"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="76" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="96" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="75" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="97" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="96" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="82" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="83" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="99" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="96" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="96" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="6">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet10"/>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="69"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="89">
+        <v>1</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="89" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="89">
+        <v>2</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="89" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="89" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="89">
+        <v>3</v>
+      </c>
+      <c r="C5" s="89" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="89" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="89" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="89">
+        <v>4</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="89" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2">
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:P28"/>
@@ -1571,7 +2698,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="85.28515625" customWidth="1"/>
@@ -1587,10 +2714,10 @@
     <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="28"/>
     </row>
-    <row r="3" spans="1:16" ht="21">
+    <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>68</v>
       </c>
@@ -1610,12 +2737,12 @@
       <c r="O3" s="41"/>
       <c r="P3" s="42"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15.75" thickBot="1">
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1630,7 +2757,7 @@
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" thickBot="1">
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -1653,7 +2780,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="28" t="s">
         <v>78</v>
       </c>
@@ -1667,12 +2794,12 @@
       </c>
       <c r="I7" s="28"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="31" t="s">
         <v>135</v>
       </c>
@@ -1689,12 +2816,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E13" s="25" t="s">
         <v>138</v>
       </c>
@@ -1708,7 +2835,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15.75" thickBot="1">
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
         <v>80</v>
       </c>
@@ -1716,7 +2843,7 @@
       <c r="C18" s="44"/>
       <c r="D18" s="44"/>
     </row>
-    <row r="19" spans="1:16" ht="15.75" thickBot="1">
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="36" t="s">
         <v>81</v>
       </c>
@@ -1730,7 +2857,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>82</v>
       </c>
@@ -1744,7 +2871,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>82</v>
       </c>
@@ -1758,7 +2885,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="21">
+    <row r="25" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
         <v>99</v>
       </c>
@@ -1778,12 +2905,12 @@
       <c r="O25" s="41"/>
       <c r="P25" s="42"/>
     </row>
-    <row r="27" spans="1:16" ht="15.75" thickBot="1">
+    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" thickBot="1">
+    <row r="28" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="35" t="s">
         <v>141</v>
       </c>
@@ -1804,18 +2931,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3">
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A2:S23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:19" ht="21.75" thickBot="1">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
         <v>25</v>
       </c>
@@ -1835,7 +2962,7 @@
       <c r="O3" s="46"/>
       <c r="P3" s="47"/>
     </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1">
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1853,7 +2980,7 @@
       <c r="R5" s="49"/>
       <c r="S5" s="50"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1871,7 +2998,7 @@
       <c r="R6" s="52"/>
       <c r="S6" s="53"/>
     </row>
-    <row r="7" spans="1:19" ht="15" customHeight="1">
+    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I7" s="54" t="s">
         <v>26</v>
       </c>
@@ -1886,7 +3013,7 @@
       <c r="R7" s="55"/>
       <c r="S7" s="56"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1904,7 +3031,7 @@
       <c r="R10" s="49"/>
       <c r="S10" s="50"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1922,7 +3049,7 @@
       <c r="R11" s="52"/>
       <c r="S11" s="53"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I12" s="54" t="s">
         <v>26</v>
       </c>
@@ -1937,7 +3064,7 @@
       <c r="R12" s="55"/>
       <c r="S12" s="56"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1955,7 +3082,7 @@
       <c r="R15" s="49"/>
       <c r="S15" s="50"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I16" s="51"/>
       <c r="J16" s="52"/>
       <c r="K16" s="52"/>
@@ -1968,7 +3095,7 @@
       <c r="R16" s="52"/>
       <c r="S16" s="53"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1984,12 +3111,12 @@
       <c r="R17" s="55"/>
       <c r="S17" s="56"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -2010,7 +3137,7 @@
       <c r="R21" s="49"/>
       <c r="S21" s="50"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I22" s="51"/>
       <c r="J22" s="52"/>
       <c r="K22" s="52"/>
@@ -2023,7 +3150,7 @@
       <c r="R22" s="52"/>
       <c r="S22" s="53"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2057,8 +3184,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4">
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A3:Q73"/>
@@ -2067,7 +3194,7 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
@@ -2078,7 +3205,7 @@
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" ht="21">
+    <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>88</v>
       </c>
@@ -2098,7 +3225,7 @@
       <c r="O3" s="41"/>
       <c r="P3" s="42"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>0</v>
       </c>
@@ -2118,12 +3245,12 @@
       <c r="O4" s="61"/>
       <c r="P4" s="62"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
@@ -2140,7 +3267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
         <v>2</v>
       </c>
@@ -2160,12 +3287,12 @@
       <c r="O8" s="61"/>
       <c r="P8" s="62"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2182,7 +3309,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>28</v>
@@ -2197,7 +3324,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -2211,7 +3338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="s">
         <v>6</v>
       </c>
@@ -2231,12 +3358,12 @@
       <c r="O15" s="61"/>
       <c r="P15" s="62"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -2247,7 +3374,7 @@
       <c r="D17" s="64"/>
       <c r="E17" s="65"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2264,7 +3391,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
         <v>64</v>
@@ -2279,7 +3406,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -2290,7 +3417,7 @@
       <c r="D20" s="64"/>
       <c r="E20" s="65"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -2304,7 +3431,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="21">
+    <row r="26" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
         <v>89</v>
       </c>
@@ -2324,7 +3451,7 @@
       <c r="O26" s="41"/>
       <c r="P26" s="42"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="60" t="s">
         <v>90</v>
       </c>
@@ -2344,7 +3471,7 @@
       <c r="O27" s="61"/>
       <c r="P27" s="62"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>93</v>
       </c>
@@ -2358,7 +3485,7 @@
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="4" t="s">
         <v>121</v>
@@ -2376,7 +3503,7 @@
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
@@ -2388,7 +3515,7 @@
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
         <v>96</v>
       </c>
@@ -2408,7 +3535,7 @@
       <c r="O32" s="61"/>
       <c r="P32" s="62"/>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>95</v>
       </c>
@@ -2421,7 +3548,7 @@
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="3" t="s">
         <v>31</v>
@@ -2445,7 +3572,7 @@
       <c r="M34" s="15"/>
       <c r="N34" s="15"/>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>28</v>
       </c>
@@ -2468,7 +3595,7 @@
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B36" s="66" t="s">
         <v>67</v>
       </c>
@@ -2484,7 +3611,7 @@
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>122</v>
       </c>
@@ -2501,13 +3628,13 @@
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
@@ -2519,7 +3646,7 @@
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="60" t="s">
         <v>97</v>
       </c>
@@ -2539,7 +3666,7 @@
       <c r="O40" s="61"/>
       <c r="P40" s="62"/>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>91</v>
       </c>
@@ -2556,7 +3683,7 @@
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="11" t="s">
         <v>123</v>
@@ -2578,12 +3705,12 @@
       <c r="M42" s="15"/>
       <c r="N42" s="15"/>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -2594,7 +3721,7 @@
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>59</v>
       </c>
@@ -2613,7 +3740,7 @@
       <c r="N45" s="15"/>
       <c r="O45" s="15"/>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
         <v>39</v>
       </c>
@@ -2630,7 +3757,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B47" s="17"/>
       <c r="C47" s="18" t="s">
         <v>126</v>
@@ -2645,7 +3772,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>33</v>
       </c>
@@ -2660,7 +3787,7 @@
       </c>
       <c r="K48" s="4"/>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
       <c r="D49" s="16"/>
@@ -2668,10 +3795,10 @@
       <c r="F49" s="16"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>62</v>
       </c>
@@ -2683,7 +3810,7 @@
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="9" t="s">
         <v>123</v>
@@ -2698,14 +3825,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G54" s="4"/>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>54</v>
       </c>
@@ -2715,7 +3842,7 @@
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="11" t="s">
         <v>130</v>
@@ -2736,7 +3863,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>65</v>
       </c>
@@ -2746,7 +3873,7 @@
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="11" t="s">
         <v>130</v>
@@ -2761,7 +3888,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="57" t="s">
         <v>40</v>
       </c>
@@ -2773,7 +3900,7 @@
       <c r="G69" s="58"/>
       <c r="H69" s="59"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>41</v>
       </c>
@@ -2799,7 +3926,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>51</v>
       </c>
@@ -2807,7 +3934,7 @@
       <c r="F71" s="16"/>
       <c r="G71" s="16"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>57</v>
       </c>
@@ -2836,8 +3963,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5">
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A2:P6"/>
@@ -2846,9 +3973,9 @@
       <selection activeCell="B6" sqref="B6:O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:16" ht="21">
+    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>103</v>
       </c>
@@ -2868,7 +3995,7 @@
       <c r="O2" s="41"/>
       <c r="P2" s="42"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>119</v>
       </c>
@@ -2888,12 +4015,12 @@
       <c r="O4" s="61"/>
       <c r="P4" s="62"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>104</v>
       </c>
@@ -2947,4 +4074,465 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="69"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="89">
+        <v>1</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="89" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="89">
+        <v>2</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="89" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="89" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="89">
+        <v>3</v>
+      </c>
+      <c r="C5" s="89" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="89" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="89" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="89">
+        <v>4</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="89" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="69"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="90" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="90" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="90" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="90" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="89">
+        <v>1</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="89" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="89">
+        <v>2</v>
+      </c>
+      <c r="C5" s="89" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="89" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="89" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="89">
+        <v>3</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="89" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="89" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="89">
+        <v>4</v>
+      </c>
+      <c r="C7" s="89" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="89" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="92"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="93"/>
+    </row>
+  </sheetData>
+  <sheetProtection scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="69"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="93"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="90" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="90" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="90" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="89">
+        <v>1</v>
+      </c>
+      <c r="C5" s="89" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="89" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="89">
+        <v>2</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="89" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="89" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="89">
+        <v>3</v>
+      </c>
+      <c r="C7" s="89" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" s="89" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="89">
+        <v>4</v>
+      </c>
+      <c r="C8" s="89" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="89" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="93"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="93"/>
+    </row>
+  </sheetData>
+  <sheetProtection scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="3">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="69"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="94">
+        <v>1</v>
+      </c>
+      <c r="C3" s="94" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="95">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="94">
+        <v>2</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="95">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="94">
+        <v>3</v>
+      </c>
+      <c r="C5" s="94" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="95">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="94">
+        <v>4</v>
+      </c>
+      <c r="C6" s="94" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="95">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="94">
+        <v>5</v>
+      </c>
+      <c r="C7" s="94" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="95">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="94">
+        <v>6</v>
+      </c>
+      <c r="C8" s="94" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" s="95">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="94">
+        <v>7</v>
+      </c>
+      <c r="C9" s="94" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" s="95">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="94">
+        <v>8</v>
+      </c>
+      <c r="C10" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" s="95">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="94">
+        <v>9</v>
+      </c>
+      <c r="C11" s="94" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="95">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="94">
+        <v>10</v>
+      </c>
+      <c r="C12" s="94" t="s">
+        <v>176</v>
+      </c>
+      <c r="D12" s="95">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>